<commit_message>
adjusted hull 96px, paint 400px on templates
</commit_message>
<xml_diff>
--- a/templates/BoatsOnOrderTemplate.xlsx
+++ b/templates/BoatsOnOrderTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fredw\AppData\Local\Temp\scp58274\home\fwarren\.venv\smartsheet_boats_on_order\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Fred\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Boats on Order</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>Colors    Interior / Exterior</t>
+  </si>
+  <si>
+    <t>NRB27003H0</t>
   </si>
 </sst>
 </file>
@@ -1090,16 +1093,18 @@
     <tabColor rgb="FF00B0F0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N2007"/>
+  <dimension ref="A1:L2007"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="7" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" style="2" customWidth="1"/>
     <col min="2" max="2" width="32.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="40.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="59.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="17" style="2" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" style="7" customWidth="1"/>
     <col min="7" max="7" width="17.28515625" style="4" customWidth="1"/>
@@ -1208,7 +1213,9 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="12" x14ac:dyDescent="0.2">
-      <c r="A9"/>
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
       <c r="B9"/>
       <c r="C9"/>
       <c r="D9"/>
@@ -21204,7 +21211,7 @@
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="78" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup scale="70" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
adjusted paint 512px, engine 160px  on templates
</commit_message>
<xml_diff>
--- a/templates/BoatsOnOrderTemplate.xlsx
+++ b/templates/BoatsOnOrderTemplate.xlsx
@@ -1095,17 +1095,15 @@
   </sheetPr>
   <dimension ref="A1:L2007"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.28515625" style="2" customWidth="1"/>
     <col min="2" max="2" width="32.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="59.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="17" style="2" customWidth="1"/>
+    <col min="4" max="4" width="76.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" style="2" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" style="7" customWidth="1"/>
     <col min="7" max="7" width="17.28515625" style="4" customWidth="1"/>
     <col min="8" max="8" width="33.42578125" style="4" customWidth="1"/>
@@ -21211,7 +21209,7 @@
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="70" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup scale="63" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
adjusted engine 212px  on templates
</commit_message>
<xml_diff>
--- a/templates/BoatsOnOrderTemplate.xlsx
+++ b/templates/BoatsOnOrderTemplate.xlsx
@@ -1095,7 +1095,9 @@
   </sheetPr>
   <dimension ref="A1:L2007"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1103,7 +1105,7 @@
     <col min="2" max="2" width="32.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" style="3" customWidth="1"/>
     <col min="4" max="4" width="76.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="31" style="2" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" style="7" customWidth="1"/>
     <col min="7" max="7" width="17.28515625" style="4" customWidth="1"/>
     <col min="8" max="8" width="33.42578125" style="4" customWidth="1"/>
@@ -21209,7 +21211,7 @@
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="63" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup scale="61" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
adjusted engine 232px  on templates
</commit_message>
<xml_diff>
--- a/templates/BoatsOnOrderTemplate.xlsx
+++ b/templates/BoatsOnOrderTemplate.xlsx
@@ -1095,9 +1095,7 @@
   </sheetPr>
   <dimension ref="A1:L2007"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1105,7 +1103,7 @@
     <col min="2" max="2" width="32.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" style="3" customWidth="1"/>
     <col min="4" max="4" width="76.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="31" style="2" customWidth="1"/>
+    <col min="5" max="5" width="34.5703125" style="2" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" style="7" customWidth="1"/>
     <col min="7" max="7" width="17.28515625" style="4" customWidth="1"/>
     <col min="8" max="8" width="33.42578125" style="4" customWidth="1"/>
@@ -21211,7 +21209,7 @@
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="61" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup scale="60" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>

</xml_diff>